<commit_message>
deleting samples with no fastq file; updated fastq08.02.19 to correct the fastq file names
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_J.PLAGGENBERG_08.02.19.xlsx
+++ b/fastqFiles/fastq_J.PLAGGENBERG_08.02.19.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/fastqFiles/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC63558D-30FB-6F4C-94AC-D4A6F9D8A993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="140" yWindow="600" windowWidth="21580" windowHeight="19080" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -20,359 +33,376 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="96">
-  <si>
-    <t xml:space="preserve">libraryDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libraryPreparer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">librarySampleNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">runNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">laneNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequencerModel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flowcellType</t>
-  </si>
-  <si>
-    <t xml:space="preserve">purpose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tapestationConc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">volumePooled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">readsObtained</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fastqFileName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06.03.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.PLAGGENBERG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NextSeq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HighOutput</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fullRNASeq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_2_GTAC_2_SIC_Index2_10_GCTTAGA_GCTTCT_S2_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_3_GTAC_3_SIC_Index2_10_ATGACAG_GCTTCT_S3_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_5_GTAC_5_SIC_Index2_10_ATCGAGC_GCTTCT_S4_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_6_GTAC_6_SIC_Index2_10_TACTCTA_GCTTCT_S5_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_7_GTAC_7_SIC_Index2_10_AGACTGA_GCTTCT_S6_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_10_GTAC_11_SIC_Index2_10_CCATCAT_GCTTCT_S7_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_11_GTAC_12_SIC_Index2_10_TAACAAG_GCTTCT_S8_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_12_GTAC_13_SIC_Index2_10_GAGGCGT_GCTTCT_S9_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_13_GTAC_14_SIC_Index2_10_TTTAACT_GCTTCT_S10_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_14_GTAC_15_SIC_Index2_10_GGTCCTC_GCTTCT_S11_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_15_GTAC_16_SIC_Index2_10_CGGTGGC_GCTTCT_S12_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_16_GTAC_17_SIC_Index2_10_ACTGTCG_GCTTCT_S13_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_21_GTAC_22_SIC_Index2_10_AAATGCA_GCTTCT_S14_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_22_GTAC_23_SIC_Index2_10_ACGCGGG_GCTTCT_S15_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_25_GTAC_26_SIC_Index2_10_TCAACTG_GCTTCT_S16_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_29_GTAC_39_SIC_Index2_10_CCGGACC_GCTTCT_S17_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06.17.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_1_GTAC_47_SIC_Index2_6_ATGTTCT_GACCTT_S24_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_2_GTAC_48_SIC_Index2_6_GTAAAAA_GACCTT_S25_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_3_GTAC_49_SIC_Index2_6_GTCTGAT_GACCTT_S26_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_5_GTAC_51_SIC_Index2_6_CTCCCGA_GACCTT_S27_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_6_GTAC_52_SIC_Index2_6_GCCGTTT_GACCTT_S28_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_7_GTAC_53_SIC_Index2_6_TAGGTAA_GACCTT_S29_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_8_GTAC_54_SIC_Index2_6_TCGAGAT_GACCTT_S30_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_10_GTAC_56_SIC_Index2_6_TCCGGGA_GACCTT_S31_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_13_GTAC_59_SIC_Index2_6_AGTTATG_GACCTT_S32_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_14_GTAC_60_SIC_Index2_6_CTGCAAT_GACCTT_S33_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_15_GTAC_61_SIC_Index2_6_CAAGCCG_GACCTT_S34_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_16_GTAC_62_SIC_Index2_6_GGGTCAA_GACCTT_S35_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_17_GTAC_63_SIC_Index2_6_GCAACGC_GACCTT_S36_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_18_GTAC_64_SIC_Index2_6_TGATTAC_GACCTT_S37_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_19_GTAC_65_SIC_Index2_6_TGCTGGG_GACCTT_S38_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_30_GTAC_11_SIC_Index2_6_CCATCAT_GACCTT_S47_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_31_GTAC_12_SIC_Index2_6_TAACAAG_GACCTT_S48_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_32_GTAC_13_SIC_Index2_6_GAGGCGT_GACCTT_S49_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_34_GTAC_15_SIC_Index2_6_GGTCCTC_GACCTT_S50_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07.01.19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_2_GTAC_2_SIC_Index_7_GCTTAGA_GAGTTG_S51_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_5_GTAC_5_SIC_Index_7_ATCGAGC_GAGTTG_S52_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_6_GTAC_6_SIC_Index_7_TACTCTA_GAGTTG_S53_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H.BROWN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_26_GTAC_26_SIC_Index_7_TCAACTG_GAGTTG_S54_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_27_GTAC_27_SIC_Index_7_TGTTTGT_GAGTTG_S55_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_28_GTAC_28_SIC_Index_7_TACATGG_GAGTTG_S56_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_29_GTAC_29_SIC_Index_7_GTTCTCA_GAGTTG_S57_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_30_GTAC_30_SIC_Index_7_CTGGTGG_GAGTTG_S58_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_7_GTAC_7_SIC_Index_7_AGACTGA_GAGTTG_S59_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_8_GTAC_8_SIC_Index_7_CTTGGAA_GAGTTG_S60_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_9_GTAC_9_SIC_Index_7_CCGATTA_GAGTTG_S61_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_10_GTAC_10_SIC_Index_7_GGCAGCG_GAGTTG_S62_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_11_GTAC_11_SIC_Index_7_CCATCAT_GAGTTG_S63_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_12_GTAC_12_SIC_Index_7_TAACAAG_GAGTTG_S64_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_32_GTAC_32_SIC_Index_7_AAACCTT_GAGTTG_S65_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_33_GTAC_33_SIC_Index_7_ACCATAC_GAGTTG_S66_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_34_GTAC_34_SIC_Index_7_AATACGC_GAGTTG_S67_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_35_GTAC_35_SIC_Index_7_CGCTACA_GAGTTG_S68_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_36_GTAC_36_SIC_Index_7_TGGCATA_GAGTTG_S69_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_13_GTAC_13_SIC_Index_7_GAGGCGT_GAGTTG_S70_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_14_GTAC_14_SIC_Index_7_TTTAACT_GAGTTG_S71_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_15_GTAC_15_SIC_Index_7_GGTCCTC_GAGTTG_S72_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_16_GTAC_16_SIC_Index_7_CGGTGGC_GAGTTG_S73_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_17_GTAC_17_SIC_Index_7_ACTGTCG_GAGTTG_S74_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_18_GTAC_18_SIC_Index_7_GTATTTG_GAGTTG_S75_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_37_GTAC_37_SIC_Index_7_TTTTGTC_GAGTTG_S76_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_38_GTAC_38_SIC_Index_7_ACCCACT_GAGTTG_S77_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_39_GTAC_39_SIC_Index_7_CCGGACC_GAGTTG_S78_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_40_GTAC_40_SIC_Index_7_GTACGGC_GAGTTG_S79_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_42_GTAC_42_SIC_Index_7_ACTCCAA_GAGTTG_S80_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_19_GTAC_19_SIC_Index_7_GAGTACG_GAGTTG_S81_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_20_GTAC_20_SIC_Index_7_ACAGATA_GAGTTG_S82_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_22_GTAC_22_SIC_Index_7_AAATGCA_GAGTTG_S83_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_23_GTAC_23_SIC_Index_7_ACGCGGG_GAGTTG_S84_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_24_GTAC_24_SIC_Index_7_GGAGTCC_GAGTTG_S85_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_43_GTAC_43_SIC_Index_7_TGTGCCA_GAGTTG_S86_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_44_GTAC_44_SIC_Index_7_AACGGAG_GAGTTG_S87_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_45_GTAC_45_SIC_Index_7_GATAGTT_GAGTTG_S88_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_46_GTAC_46_SIC_Index_7_GGTGAAT_GAGTTG_S89_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_47_GTAC_47_SIC_Index_7_ATGTTCT_GAGTTG_S90_R1_001.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_48_GTAC_48_SIC_Index_7_GTAAAAA_GAGTTG_S91_R1_001.fastq.gz</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="110">
+  <si>
+    <t>libraryDate</t>
+  </si>
+  <si>
+    <t>libraryPreparer</t>
+  </si>
+  <si>
+    <t>librarySampleNumber</t>
+  </si>
+  <si>
+    <t>runNumber</t>
+  </si>
+  <si>
+    <t>laneNumber</t>
+  </si>
+  <si>
+    <t>sequencerModel</t>
+  </si>
+  <si>
+    <t>flowcellType</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>tapestationConc</t>
+  </si>
+  <si>
+    <t>volumePooled</t>
+  </si>
+  <si>
+    <t>readsObtained</t>
+  </si>
+  <si>
+    <t>fastqFileName</t>
+  </si>
+  <si>
+    <t>06.03.19</t>
+  </si>
+  <si>
+    <t>J.PLAGGENBERG</t>
+  </si>
+  <si>
+    <t>NextSeq</t>
+  </si>
+  <si>
+    <t>HighOutput</t>
+  </si>
+  <si>
+    <t>fullRNASeq</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_2_GTAC_2_SIC_Index2_10_GCTTAGA_GCTTCT_S2_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_3_GTAC_3_SIC_Index2_10_ATGACAG_GCTTCT_S3_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_5_GTAC_5_SIC_Index2_10_ATCGAGC_GCTTCT_S4_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_6_GTAC_6_SIC_Index2_10_TACTCTA_GCTTCT_S5_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_7_GTAC_7_SIC_Index2_10_AGACTGA_GCTTCT_S6_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_10_GTAC_11_SIC_Index2_10_CCATCAT_GCTTCT_S7_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_11_GTAC_12_SIC_Index2_10_TAACAAG_GCTTCT_S8_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_12_GTAC_13_SIC_Index2_10_GAGGCGT_GCTTCT_S9_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_13_GTAC_14_SIC_Index2_10_TTTAACT_GCTTCT_S10_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_14_GTAC_15_SIC_Index2_10_GGTCCTC_GCTTCT_S11_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_15_GTAC_16_SIC_Index2_10_CGGTGGC_GCTTCT_S12_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_16_GTAC_17_SIC_Index2_10_ACTGTCG_GCTTCT_S13_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_21_GTAC_22_SIC_Index2_10_AAATGCA_GCTTCT_S14_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_22_GTAC_23_SIC_Index2_10_ACGCGGG_GCTTCT_S15_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_25_GTAC_26_SIC_Index2_10_TCAACTG_GCTTCT_S16_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_29_GTAC_39_SIC_Index2_10_CCGGACC_GCTTCT_S17_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>06.17.19</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_1_GTAC_47_SIC_Index2_6_ATGTTCT_GACCTT_S24_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_2_GTAC_48_SIC_Index2_6_GTAAAAA_GACCTT_S25_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_3_GTAC_49_SIC_Index2_6_GTCTGAT_GACCTT_S26_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_5_GTAC_51_SIC_Index2_6_CTCCCGA_GACCTT_S27_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_6_GTAC_52_SIC_Index2_6_GCCGTTT_GACCTT_S28_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_7_GTAC_53_SIC_Index2_6_TAGGTAA_GACCTT_S29_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_8_GTAC_54_SIC_Index2_6_TCGAGAT_GACCTT_S30_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_10_GTAC_56_SIC_Index2_6_TCCGGGA_GACCTT_S31_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_13_GTAC_59_SIC_Index2_6_AGTTATG_GACCTT_S32_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_14_GTAC_60_SIC_Index2_6_CTGCAAT_GACCTT_S33_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_15_GTAC_61_SIC_Index2_6_CAAGCCG_GACCTT_S34_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_16_GTAC_62_SIC_Index2_6_GGGTCAA_GACCTT_S35_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_17_GTAC_63_SIC_Index2_6_GCAACGC_GACCTT_S36_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_18_GTAC_64_SIC_Index2_6_TGATTAC_GACCTT_S37_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_19_GTAC_65_SIC_Index2_6_TGCTGGG_GACCTT_S38_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_30_GTAC_11_SIC_Index2_6_CCATCAT_GACCTT_S47_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_31_GTAC_12_SIC_Index2_6_TAACAAG_GACCTT_S48_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_32_GTAC_13_SIC_Index2_6_GAGGCGT_GACCTT_S49_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_34_GTAC_15_SIC_Index2_6_GGTCCTC_GACCTT_S50_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>07.01.19</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_2_GTAC_2_SIC_Index_7_GCTTAGA_GAGTTG_S51_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_5_GTAC_5_SIC_Index_7_ATCGAGC_GAGTTG_S52_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_6_GTAC_6_SIC_Index_7_TACTCTA_GAGTTG_S53_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>H.BROWN</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_26_GTAC_26_SIC_Index_7_TCAACTG_GAGTTG_S54_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_27_GTAC_27_SIC_Index_7_TGTTTGT_GAGTTG_S55_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_28_GTAC_28_SIC_Index_7_TACATGG_GAGTTG_S56_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_29_GTAC_29_SIC_Index_7_GTTCTCA_GAGTTG_S57_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_30_GTAC_30_SIC_Index_7_CTGGTGG_GAGTTG_S58_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_7_GTAC_7_SIC_Index_7_AGACTGA_GAGTTG_S59_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_8_GTAC_8_SIC_Index_7_CTTGGAA_GAGTTG_S60_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_9_GTAC_9_SIC_Index_7_CCGATTA_GAGTTG_S61_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_10_GTAC_10_SIC_Index_7_GGCAGCG_GAGTTG_S62_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_11_GTAC_11_SIC_Index_7_CCATCAT_GAGTTG_S63_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_12_GTAC_12_SIC_Index_7_TAACAAG_GAGTTG_S64_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_32_GTAC_32_SIC_Index_7_AAACCTT_GAGTTG_S65_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_33_GTAC_33_SIC_Index_7_ACCATAC_GAGTTG_S66_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_34_GTAC_34_SIC_Index_7_AATACGC_GAGTTG_S67_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_35_GTAC_35_SIC_Index_7_CGCTACA_GAGTTG_S68_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_36_GTAC_36_SIC_Index_7_TGGCATA_GAGTTG_S69_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_13_GTAC_13_SIC_Index_7_GAGGCGT_GAGTTG_S70_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_14_GTAC_14_SIC_Index_7_TTTAACT_GAGTTG_S71_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_15_GTAC_15_SIC_Index_7_GGTCCTC_GAGTTG_S72_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_16_GTAC_16_SIC_Index_7_CGGTGGC_GAGTTG_S73_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_17_GTAC_17_SIC_Index_7_ACTGTCG_GAGTTG_S74_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_18_GTAC_18_SIC_Index_7_GTATTTG_GAGTTG_S75_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_37_GTAC_37_SIC_Index_7_TTTTGTC_GAGTTG_S76_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_38_GTAC_38_SIC_Index_7_ACCCACT_GAGTTG_S77_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_39_GTAC_39_SIC_Index_7_CCGGACC_GAGTTG_S78_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_40_GTAC_40_SIC_Index_7_GTACGGC_GAGTTG_S79_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_42_GTAC_42_SIC_Index_7_ACTCCAA_GAGTTG_S80_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_19_GTAC_19_SIC_Index_7_GAGTACG_GAGTTG_S81_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_20_GTAC_20_SIC_Index_7_ACAGATA_GAGTTG_S82_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_22_GTAC_22_SIC_Index_7_AAATGCA_GAGTTG_S83_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_23_GTAC_23_SIC_Index_7_ACGCGGG_GAGTTG_S84_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_24_GTAC_24_SIC_Index_7_GGAGTCC_GAGTTG_S85_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_43_GTAC_43_SIC_Index_7_TGTGCCA_GAGTTG_S86_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_44_GTAC_44_SIC_Index_7_AACGGAG_GAGTTG_S87_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_45_GTAC_45_SIC_Index_7_GATAGTT_GAGTTG_S88_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_46_GTAC_46_SIC_Index_7_GGTGAAT_GAGTTG_S89_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_47_GTAC_47_SIC_Index_7_ATGTTCT_GAGTTG_S90_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep3_Rep3_48_GTAC_48_SIC_Index_7_GTAAAAA_GAGTTG_S91_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_30_GTAC_40_SIC_Index2_10_GTACGGC_GCTTCT_S18_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_31_GTAC_41_SIC_Index2_10_TTGCCCC_GCTTCT_S19_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_32_GTAC_42_SIC_Index2_10_ACTCCAA_GCTTCT_S20_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_33_GTAC_43_SIC_Index2_10_TGTGCCA_GCTTCT_S21_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_34_GTAC_44_SIC_Index2_10_AACGGAG_GCTTCT_S22_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep1_Rep1_35_GTAC_45_SIC_Index2_10_GATAGTT_GCTTCT_S23_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_20_GTAC_66_SIC_Index2_6_GACACAG_GACCTT_S39_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_23_GTAC_3_SIC_Index2_6_ATGACAG_GACCTT_S40_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_24_GTAC_4_SIC_Index2_6_CACCTCC_GACCTT_S41_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_25_GTAC_5_SIC_Index2_6_ATCGAGC_GACCTT_S42_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_26_GTAC_6_SIC_Index2_6_TACTCTA_GACCTT_S43_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_27_GTAC_7_SIC_Index2_6_AGACTGA_GACCTT_S44_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_28_GTAC_9_SIC_Index2_6_CCGATTA_GACCTT_S45_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>3766_Brent_ZEV_FloodDelayExpB_Rep2_Rep2_29_GTAC_10_SIC_Index2_6_GGCAGCG_GACCTT_S46_R1_001.fastq.gz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0"/>
-  </numFmts>
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -385,8 +415,13 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -398,7 +433,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -406,85 +441,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -543,30 +531,342 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A93" activeCellId="0" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="83.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="14.5"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" customWidth="1"/>
+    <col min="4" max="4" width="0.83203125" customWidth="1"/>
+    <col min="5" max="11" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="83.83203125" customWidth="1"/>
+    <col min="13" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -618,17 +918,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>3766</v>
       </c>
       <c r="E2" s="1"/>
@@ -641,13 +941,13 @@
       <c r="H2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="3">
         <v>21.7</v>
       </c>
-      <c r="J2" s="3" t="n">
-        <v>0.702993260970912</v>
-      </c>
-      <c r="K2" s="6" t="n">
+      <c r="J2" s="3">
+        <v>0.70299326097091197</v>
+      </c>
+      <c r="K2" s="6">
         <v>817845</v>
       </c>
       <c r="L2" s="7" t="s">
@@ -668,17 +968,17 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="3">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="4">
         <v>3766</v>
       </c>
       <c r="E3" s="1"/>
@@ -691,13 +991,13 @@
       <c r="H3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="3">
         <v>15.3</v>
       </c>
-      <c r="J3" s="3" t="n">
-        <v>0.729794206634529</v>
-      </c>
-      <c r="K3" s="6" t="n">
+      <c r="J3" s="3">
+        <v>0.72979420663452899</v>
+      </c>
+      <c r="K3" s="6">
         <v>885268</v>
       </c>
       <c r="L3" s="7" t="s">
@@ -718,17 +1018,17 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="4">
         <v>3766</v>
       </c>
       <c r="E4" s="1"/>
@@ -741,13 +1041,13 @@
       <c r="H4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="3" t="n">
-        <v>19.4</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>0.855279744069581</v>
-      </c>
-      <c r="K4" s="6" t="n">
+      <c r="I4" s="3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.85527974406958096</v>
+      </c>
+      <c r="K4" s="6">
         <v>777276</v>
       </c>
       <c r="L4" s="7" t="s">
@@ -768,17 +1068,17 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="4">
         <v>3766</v>
       </c>
       <c r="E5" s="1"/>
@@ -791,13 +1091,13 @@
       <c r="H5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="3">
         <v>30.2</v>
       </c>
-      <c r="J5" s="3" t="n">
-        <v>0.609199891483377</v>
-      </c>
-      <c r="K5" s="6" t="n">
+      <c r="J5" s="3">
+        <v>0.60919989148337705</v>
+      </c>
+      <c r="K5" s="6">
         <v>915982</v>
       </c>
       <c r="L5" s="7" t="s">
@@ -818,17 +1118,17 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="3">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="4">
         <v>3766</v>
       </c>
       <c r="E6" s="1"/>
@@ -841,13 +1141,13 @@
       <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="3">
         <v>1.08</v>
       </c>
-      <c r="J6" s="3" t="n">
-        <v>19.1007197616925</v>
-      </c>
-      <c r="K6" s="6" t="n">
+      <c r="J6" s="3">
+        <v>19.100719761692499</v>
+      </c>
+      <c r="K6" s="6">
         <v>2776308</v>
       </c>
       <c r="L6" s="7" t="s">
@@ -868,17 +1168,17 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="3">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="4">
         <v>3766</v>
       </c>
       <c r="E7" s="1"/>
@@ -891,13 +1191,13 @@
       <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="3">
         <v>29.5</v>
       </c>
-      <c r="J7" s="3" t="n">
-        <v>0.829956586315879</v>
-      </c>
-      <c r="K7" s="6" t="n">
+      <c r="J7" s="3">
+        <v>0.82995658631587899</v>
+      </c>
+      <c r="K7" s="6">
         <v>2839147</v>
       </c>
       <c r="L7" s="7" t="s">
@@ -918,17 +1218,17 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="3">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="4">
         <v>3766</v>
       </c>
       <c r="E8" s="1"/>
@@ -941,13 +1241,13 @@
       <c r="H8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="3" t="n">
+      <c r="I8" s="3">
         <v>22.8</v>
       </c>
-      <c r="J8" s="3" t="n">
-        <v>0.904352227982634</v>
-      </c>
-      <c r="K8" s="6" t="n">
+      <c r="J8" s="3">
+        <v>0.90435222798263404</v>
+      </c>
+      <c r="K8" s="6">
         <v>790391</v>
       </c>
       <c r="L8" s="7" t="s">
@@ -968,17 +1268,17 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="4">
         <v>3766</v>
       </c>
       <c r="E9" s="1"/>
@@ -991,13 +1291,13 @@
       <c r="H9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="3" t="n">
+      <c r="I9" s="3">
         <v>44.3</v>
       </c>
-      <c r="J9" s="3" t="n">
-        <v>0.676202116482027</v>
-      </c>
-      <c r="K9" s="6" t="n">
+      <c r="J9" s="3">
+        <v>0.67620211648202699</v>
+      </c>
+      <c r="K9" s="6">
         <v>832208</v>
       </c>
       <c r="L9" s="7" t="s">
@@ -1018,17 +1318,17 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4" t="n">
+      <c r="C10" s="3">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4">
         <v>3766</v>
       </c>
       <c r="E10" s="1"/>
@@ -1041,13 +1341,13 @@
       <c r="H10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="3" t="n">
+      <c r="I10" s="3">
         <v>65.8</v>
       </c>
-      <c r="J10" s="3" t="n">
-        <v>0.563593188836206</v>
-      </c>
-      <c r="K10" s="6" t="n">
+      <c r="J10" s="3">
+        <v>0.56359318883620602</v>
+      </c>
+      <c r="K10" s="6">
         <v>684109</v>
       </c>
       <c r="L10" s="7" t="s">
@@ -1068,17 +1368,17 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="3" t="n">
-        <v>14</v>
-      </c>
-      <c r="D11" s="4" t="n">
+      <c r="C11" s="3">
+        <v>14</v>
+      </c>
+      <c r="D11" s="4">
         <v>3766</v>
       </c>
       <c r="E11" s="1"/>
@@ -1091,13 +1391,13 @@
       <c r="H11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="3" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="J11" s="3" t="n">
-        <v>0.365597316417286</v>
-      </c>
-      <c r="K11" s="6" t="n">
+      <c r="I11" s="3">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.36559731641728599</v>
+      </c>
+      <c r="K11" s="6">
         <v>1028503</v>
       </c>
       <c r="L11" s="7" t="s">
@@ -1118,17 +1418,17 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="3" t="n">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="n">
+      <c r="C12" s="3">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4">
         <v>3766</v>
       </c>
       <c r="E12" s="1"/>
@@ -1141,13 +1441,13 @@
       <c r="H12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="3" t="n">
+      <c r="I12" s="3">
         <v>59.6</v>
       </c>
-      <c r="J12" s="3" t="n">
-        <v>0.589844429806371</v>
-      </c>
-      <c r="K12" s="6" t="n">
+      <c r="J12" s="3">
+        <v>0.58984442980637097</v>
+      </c>
+      <c r="K12" s="6">
         <v>521147</v>
       </c>
       <c r="L12" s="7" t="s">
@@ -1168,17 +1468,17 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="D13" s="4" t="n">
+      <c r="C13" s="3">
+        <v>16</v>
+      </c>
+      <c r="D13" s="4">
         <v>3766</v>
       </c>
       <c r="E13" s="1"/>
@@ -1191,13 +1491,13 @@
       <c r="H13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="3" t="n">
+      <c r="I13" s="3">
         <v>42.3</v>
       </c>
-      <c r="J13" s="3" t="n">
-        <v>0.660620732871372</v>
-      </c>
-      <c r="K13" s="6" t="n">
+      <c r="J13" s="3">
+        <v>0.66062073287137202</v>
+      </c>
+      <c r="K13" s="6">
         <v>819282</v>
       </c>
       <c r="L13" s="7" t="s">
@@ -1218,17 +1518,17 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="3">
         <v>21</v>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="4">
         <v>3766</v>
       </c>
       <c r="E14" s="1"/>
@@ -1241,13 +1541,13 @@
       <c r="H14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="3" t="n">
+      <c r="I14" s="3">
         <v>8.32</v>
       </c>
-      <c r="J14" s="3" t="n">
+      <c r="J14" s="3">
         <v>0.696073607200967</v>
       </c>
-      <c r="K14" s="6" t="n">
+      <c r="K14" s="6">
         <v>719974</v>
       </c>
       <c r="L14" s="7" t="s">
@@ -1268,17 +1568,17 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="3">
         <v>22</v>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="4">
         <v>3766</v>
       </c>
       <c r="E15" s="1"/>
@@ -1291,13 +1591,13 @@
       <c r="H15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="3" t="n">
+      <c r="I15" s="3">
         <v>21.6</v>
       </c>
-      <c r="J15" s="3" t="n">
-        <v>0.581401910661581</v>
-      </c>
-      <c r="K15" s="6" t="n">
+      <c r="J15" s="3">
+        <v>0.58140191066158098</v>
+      </c>
+      <c r="K15" s="6">
         <v>850979</v>
       </c>
       <c r="L15" s="7" t="s">
@@ -1318,17 +1618,17 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="3">
         <v>25</v>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="4">
         <v>3766</v>
       </c>
       <c r="E16" s="1"/>
@@ -1341,13 +1641,13 @@
       <c r="H16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="3" t="n">
+      <c r="I16" s="3">
         <v>1.9</v>
       </c>
-      <c r="J16" s="3" t="n">
-        <v>11.4551213654026</v>
-      </c>
-      <c r="K16" s="6" t="n">
+      <c r="J16" s="3">
+        <v>11.455121365402601</v>
+      </c>
+      <c r="K16" s="6">
         <v>3057222</v>
       </c>
       <c r="L16" s="7" t="s">
@@ -1368,17 +1668,17 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="3">
         <v>29</v>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="4">
         <v>3766</v>
       </c>
       <c r="E17" s="1"/>
@@ -1391,13 +1691,13 @@
       <c r="H17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="3" t="n">
+      <c r="I17" s="3">
         <v>1.3</v>
       </c>
-      <c r="J17" s="3" t="n">
-        <v>19.1011090964873</v>
-      </c>
-      <c r="K17" s="6" t="n">
+      <c r="J17" s="3">
+        <v>19.101109096487299</v>
+      </c>
+      <c r="K17" s="6">
         <v>1270172</v>
       </c>
       <c r="L17" s="7" t="s">
@@ -1418,17 +1718,17 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="3">
         <v>30</v>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="4">
         <v>3766</v>
       </c>
       <c r="E18" s="1"/>
@@ -1441,17 +1741,17 @@
       <c r="H18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="3" t="n">
+      <c r="I18" s="3">
         <v>3.82</v>
       </c>
-      <c r="J18" s="3" t="n">
-        <v>2.3532336488669</v>
-      </c>
-      <c r="K18" s="6" t="n">
+      <c r="J18" s="3">
+        <v>2.3532336488669001</v>
+      </c>
+      <c r="K18" s="6">
         <v>720522</v>
       </c>
-      <c r="L18" s="7" t="s">
-        <v>17</v>
+      <c r="L18" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
@@ -1468,17 +1768,17 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="3">
         <v>31</v>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="4">
         <v>3766</v>
       </c>
       <c r="E19" s="1"/>
@@ -1491,17 +1791,17 @@
       <c r="H19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I19" s="3" t="n">
+      <c r="I19" s="3">
         <v>11.2</v>
       </c>
-      <c r="J19" s="3" t="n">
-        <v>0.762928672331984</v>
-      </c>
-      <c r="K19" s="6" t="n">
+      <c r="J19" s="3">
+        <v>0.76292867233198403</v>
+      </c>
+      <c r="K19" s="6">
         <v>573976</v>
       </c>
-      <c r="L19" s="7" t="s">
-        <v>17</v>
+      <c r="L19" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
@@ -1518,17 +1818,17 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="3">
         <v>32</v>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="4">
         <v>3766</v>
       </c>
       <c r="E20" s="1"/>
@@ -1541,17 +1841,17 @@
       <c r="H20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="3" t="n">
+      <c r="I20" s="3">
         <v>34.4</v>
       </c>
-      <c r="J20" s="3" t="n">
-        <v>1.47237497843143</v>
-      </c>
-      <c r="K20" s="6" t="n">
+      <c r="J20" s="3">
+        <v>1.4723749784314299</v>
+      </c>
+      <c r="K20" s="6">
         <v>791242</v>
       </c>
-      <c r="L20" s="7" t="s">
-        <v>17</v>
+      <c r="L20" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
@@ -1568,17 +1868,17 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3">
         <v>33</v>
       </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="4">
         <v>3766</v>
       </c>
       <c r="E21" s="1"/>
@@ -1591,17 +1891,17 @@
       <c r="H21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I21" s="3" t="n">
+      <c r="I21" s="3">
         <v>34.4</v>
       </c>
-      <c r="J21" s="3" t="n">
-        <v>1.01908732115735</v>
-      </c>
-      <c r="K21" s="6" t="n">
+      <c r="J21" s="3">
+        <v>1.0190873211573499</v>
+      </c>
+      <c r="K21" s="6">
         <v>941506</v>
       </c>
-      <c r="L21" s="7" t="s">
-        <v>17</v>
+      <c r="L21" s="11" t="s">
+        <v>99</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -1618,17 +1918,17 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="3">
         <v>34</v>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="4">
         <v>3766</v>
       </c>
       <c r="E22" s="1"/>
@@ -1641,17 +1941,17 @@
       <c r="H22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="3" t="n">
+      <c r="I22" s="3">
         <v>48.2</v>
       </c>
-      <c r="J22" s="3" t="n">
-        <v>0.68262855389631</v>
-      </c>
-      <c r="K22" s="6" t="n">
+      <c r="J22" s="3">
+        <v>0.68262855389631005</v>
+      </c>
+      <c r="K22" s="6">
         <v>801561</v>
       </c>
-      <c r="L22" s="7" t="s">
-        <v>17</v>
+      <c r="L22" s="11" t="s">
+        <v>100</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1668,17 +1968,17 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="3">
         <v>35</v>
       </c>
-      <c r="D23" s="4" t="n">
+      <c r="D23" s="4">
         <v>3766</v>
       </c>
       <c r="E23" s="1"/>
@@ -1691,17 +1991,17 @@
       <c r="H23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I23" s="3" t="n">
+      <c r="I23" s="3">
         <v>75</v>
       </c>
-      <c r="J23" s="3" t="n">
-        <v>0.71532308250663</v>
-      </c>
-      <c r="K23" s="6" t="n">
+      <c r="J23" s="3">
+        <v>0.71532308250663001</v>
+      </c>
+      <c r="K23" s="6">
         <v>764101</v>
       </c>
-      <c r="L23" s="7" t="s">
-        <v>17</v>
+      <c r="L23" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1718,17 +2018,17 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="8" t="n">
+      <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="D24" s="4" t="n">
+      <c r="D24" s="4">
         <v>3766</v>
       </c>
       <c r="E24" s="1"/>
@@ -1741,13 +2041,13 @@
       <c r="H24" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="3" t="n">
+      <c r="I24" s="3">
         <v>8.16</v>
       </c>
-      <c r="J24" s="3" t="n">
-        <v>0.452426567664956</v>
-      </c>
-      <c r="K24" s="6" t="n">
+      <c r="J24" s="3">
+        <v>0.45242656766495598</v>
+      </c>
+      <c r="K24" s="6">
         <v>578397</v>
       </c>
       <c r="L24" s="7" t="s">
@@ -1768,17 +2068,17 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="8" t="n">
+      <c r="C25" s="8">
         <v>2</v>
       </c>
-      <c r="D25" s="4" t="n">
+      <c r="D25" s="4">
         <v>3766</v>
       </c>
       <c r="E25" s="1"/>
@@ -1791,13 +2091,13 @@
       <c r="H25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="3" t="n">
+      <c r="I25" s="3">
         <v>31.8</v>
       </c>
-      <c r="J25" s="3" t="n">
-        <v>0.781418235435312</v>
-      </c>
-      <c r="K25" s="6" t="n">
+      <c r="J25" s="3">
+        <v>0.78141823543531197</v>
+      </c>
+      <c r="K25" s="6">
         <v>654580</v>
       </c>
       <c r="L25" s="7" t="s">
@@ -1818,17 +2118,17 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="8" t="n">
+      <c r="C26" s="8">
         <v>3</v>
       </c>
-      <c r="D26" s="4" t="n">
+      <c r="D26" s="4">
         <v>3766</v>
       </c>
       <c r="E26" s="1"/>
@@ -1841,13 +2141,13 @@
       <c r="H26" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="3" t="n">
+      <c r="I26" s="3">
         <v>24.4</v>
       </c>
-      <c r="J26" s="3" t="n">
-        <v>1.14618750628709</v>
-      </c>
-      <c r="K26" s="6" t="n">
+      <c r="J26" s="3">
+        <v>1.1461875062870901</v>
+      </c>
+      <c r="K26" s="6">
         <v>529370</v>
       </c>
       <c r="L26" s="7" t="s">
@@ -1868,17 +2168,17 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="8" t="n">
+      <c r="C27" s="8">
         <v>5</v>
       </c>
-      <c r="D27" s="4" t="n">
+      <c r="D27" s="4">
         <v>3766</v>
       </c>
       <c r="E27" s="1"/>
@@ -1891,13 +2191,13 @@
       <c r="H27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="3" t="n">
+      <c r="I27" s="3">
         <v>15.2</v>
       </c>
-      <c r="J27" s="3" t="n">
-        <v>0.657458563535912</v>
-      </c>
-      <c r="K27" s="6" t="n">
+      <c r="J27" s="3">
+        <v>0.65745856353591203</v>
+      </c>
+      <c r="K27" s="6">
         <v>638921</v>
       </c>
       <c r="L27" s="7" t="s">
@@ -1918,17 +2218,17 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="8" t="n">
+      <c r="C28" s="8">
         <v>6</v>
       </c>
-      <c r="D28" s="4" t="n">
+      <c r="D28" s="4">
         <v>3766</v>
       </c>
       <c r="E28" s="1"/>
@@ -1941,13 +2241,13 @@
       <c r="H28" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="3" t="n">
+      <c r="I28" s="3">
         <v>45</v>
       </c>
-      <c r="J28" s="3" t="n">
+      <c r="J28" s="3">
         <v>0.490724291266945</v>
       </c>
-      <c r="K28" s="6" t="n">
+      <c r="K28" s="6">
         <v>551624</v>
       </c>
       <c r="L28" s="7" t="s">
@@ -1968,17 +2268,17 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="8" t="n">
+      <c r="C29" s="8">
         <v>7</v>
       </c>
-      <c r="D29" s="4" t="n">
+      <c r="D29" s="4">
         <v>3766</v>
       </c>
       <c r="E29" s="1"/>
@@ -1991,13 +2291,13 @@
       <c r="H29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I29" s="3" t="n">
+      <c r="I29" s="3">
         <v>41.3</v>
       </c>
-      <c r="J29" s="3" t="n">
-        <v>1.34002704927673</v>
-      </c>
-      <c r="K29" s="6" t="n">
+      <c r="J29" s="3">
+        <v>1.3400270492767301</v>
+      </c>
+      <c r="K29" s="6">
         <v>724894</v>
       </c>
       <c r="L29" s="7" t="s">
@@ -2018,17 +2318,17 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="8" t="n">
+      <c r="C30" s="8">
         <v>8</v>
       </c>
-      <c r="D30" s="4" t="n">
+      <c r="D30" s="4">
         <v>3766</v>
       </c>
       <c r="E30" s="1"/>
@@ -2041,13 +2341,13 @@
       <c r="H30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="3" t="n">
-        <v>18.9</v>
-      </c>
-      <c r="J30" s="3" t="n">
-        <v>0.634194194751343</v>
-      </c>
-      <c r="K30" s="6" t="n">
+      <c r="I30" s="3">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0.63419419475134298</v>
+      </c>
+      <c r="K30" s="6">
         <v>510099</v>
       </c>
       <c r="L30" s="7" t="s">
@@ -2068,17 +2368,17 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="8" t="n">
+      <c r="C31" s="8">
         <v>10</v>
       </c>
-      <c r="D31" s="4" t="n">
+      <c r="D31" s="4">
         <v>3766</v>
       </c>
       <c r="E31" s="1"/>
@@ -2091,13 +2391,13 @@
       <c r="H31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I31" s="3" t="n">
+      <c r="I31" s="3">
         <v>22.6</v>
       </c>
-      <c r="J31" s="3" t="n">
-        <v>0.641189049267044</v>
-      </c>
-      <c r="K31" s="6" t="n">
+      <c r="J31" s="3">
+        <v>0.64118904926704401</v>
+      </c>
+      <c r="K31" s="6">
         <v>374571</v>
       </c>
       <c r="L31" s="7" t="s">
@@ -2118,17 +2418,17 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="D32" s="4" t="n">
+      <c r="C32" s="8">
+        <v>13</v>
+      </c>
+      <c r="D32" s="4">
         <v>3766</v>
       </c>
       <c r="E32" s="1"/>
@@ -2141,13 +2441,13 @@
       <c r="H32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="3" t="n">
+      <c r="I32" s="3">
         <v>8.32</v>
       </c>
-      <c r="J32" s="3" t="n">
-        <v>0.659762111007143</v>
-      </c>
-      <c r="K32" s="6" t="n">
+      <c r="J32" s="3">
+        <v>0.65976211100714299</v>
+      </c>
+      <c r="K32" s="6">
         <v>320064</v>
       </c>
       <c r="L32" s="7" t="s">
@@ -2168,17 +2468,17 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="8" t="n">
-        <v>14</v>
-      </c>
-      <c r="D33" s="4" t="n">
+      <c r="C33" s="8">
+        <v>14</v>
+      </c>
+      <c r="D33" s="4">
         <v>3766</v>
       </c>
       <c r="E33" s="1"/>
@@ -2191,13 +2491,13 @@
       <c r="H33" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I33" s="3" t="n">
+      <c r="I33" s="3">
         <v>15.6</v>
       </c>
-      <c r="J33" s="3" t="n">
-        <v>0.815549789746802</v>
-      </c>
-      <c r="K33" s="6" t="n">
+      <c r="J33" s="3">
+        <v>0.81554978974680203</v>
+      </c>
+      <c r="K33" s="6">
         <v>679320</v>
       </c>
       <c r="L33" s="7" t="s">
@@ -2218,17 +2518,17 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="8" t="n">
-        <v>15</v>
-      </c>
-      <c r="D34" s="4" t="n">
+      <c r="C34" s="8">
+        <v>15</v>
+      </c>
+      <c r="D34" s="4">
         <v>3766</v>
       </c>
       <c r="E34" s="1"/>
@@ -2241,13 +2541,13 @@
       <c r="H34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="3" t="n">
+      <c r="I34" s="3">
         <v>14.7</v>
       </c>
-      <c r="J34" s="3" t="n">
+      <c r="J34" s="3">
         <v>1.14630281690141</v>
       </c>
-      <c r="K34" s="6" t="n">
+      <c r="K34" s="6">
         <v>610882</v>
       </c>
       <c r="L34" s="7" t="s">
@@ -2268,17 +2568,17 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="D35" s="4" t="n">
+      <c r="C35" s="8">
+        <v>16</v>
+      </c>
+      <c r="D35" s="4">
         <v>3766</v>
       </c>
       <c r="E35" s="1"/>
@@ -2291,13 +2591,13 @@
       <c r="H35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I35" s="3" t="n">
+      <c r="I35" s="3">
         <v>7.66</v>
       </c>
-      <c r="J35" s="3" t="n">
-        <v>0.93201754385965</v>
-      </c>
-      <c r="K35" s="6" t="n">
+      <c r="J35" s="3">
+        <v>0.93201754385964997</v>
+      </c>
+      <c r="K35" s="6">
         <v>726737</v>
       </c>
       <c r="L35" s="7" t="s">
@@ -2318,17 +2618,17 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="8" t="n">
+      <c r="C36" s="8">
         <v>17</v>
       </c>
-      <c r="D36" s="4" t="n">
+      <c r="D36" s="4">
         <v>3766</v>
       </c>
       <c r="E36" s="1"/>
@@ -2341,13 +2641,13 @@
       <c r="H36" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="3" t="n">
+      <c r="I36" s="3">
         <v>17.2</v>
       </c>
-      <c r="J36" s="3" t="n">
-        <v>0.560747548567281</v>
-      </c>
-      <c r="K36" s="6" t="n">
+      <c r="J36" s="3">
+        <v>0.56074754856728104</v>
+      </c>
+      <c r="K36" s="6">
         <v>551777</v>
       </c>
       <c r="L36" s="7" t="s">
@@ -2368,17 +2668,17 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="8" t="n">
+      <c r="C37" s="8">
         <v>18</v>
       </c>
-      <c r="D37" s="4" t="n">
+      <c r="D37" s="4">
         <v>3766</v>
       </c>
       <c r="E37" s="1"/>
@@ -2391,13 +2691,13 @@
       <c r="H37" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="3" t="n">
-        <v>9.28</v>
-      </c>
-      <c r="J37" s="3" t="n">
+      <c r="I37" s="3">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="J37" s="3">
         <v>0.17311587393673</v>
       </c>
-      <c r="K37" s="6" t="n">
+      <c r="K37" s="6">
         <v>786455</v>
       </c>
       <c r="L37" s="7" t="s">
@@ -2418,17 +2718,17 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="8" t="n">
+      <c r="C38" s="8">
         <v>19</v>
       </c>
-      <c r="D38" s="4" t="n">
+      <c r="D38" s="4">
         <v>3766</v>
       </c>
       <c r="E38" s="1"/>
@@ -2441,13 +2741,13 @@
       <c r="H38" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="3" t="n">
+      <c r="I38" s="3">
         <v>13.4</v>
       </c>
-      <c r="J38" s="3" t="n">
-        <v>0.823536851995736</v>
-      </c>
-      <c r="K38" s="6" t="n">
+      <c r="J38" s="3">
+        <v>0.82353685199573601</v>
+      </c>
+      <c r="K38" s="6">
         <v>621715</v>
       </c>
       <c r="L38" s="7" t="s">
@@ -2468,17 +2768,17 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="8" t="n">
+      <c r="C39" s="8">
         <v>20</v>
       </c>
-      <c r="D39" s="4" t="n">
+      <c r="D39" s="4">
         <v>3766</v>
       </c>
       <c r="E39" s="1"/>
@@ -2491,17 +2791,17 @@
       <c r="H39" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I39" s="3" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="J39" s="3" t="n">
-        <v>0.907799864558021</v>
-      </c>
-      <c r="K39" s="6" t="n">
+      <c r="I39" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0.90779986455802097</v>
+      </c>
+      <c r="K39" s="6">
         <v>716305</v>
       </c>
-      <c r="L39" s="7" t="s">
-        <v>34</v>
+      <c r="L39" s="11" t="s">
+        <v>102</v>
       </c>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
@@ -2518,17 +2818,17 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="8" t="n">
+      <c r="C40" s="8">
         <v>23</v>
       </c>
-      <c r="D40" s="4" t="n">
+      <c r="D40" s="4">
         <v>3766</v>
       </c>
       <c r="E40" s="1"/>
@@ -2541,17 +2841,17 @@
       <c r="H40" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="3" t="n">
+      <c r="I40" s="3">
         <v>3.72</v>
       </c>
-      <c r="J40" s="3" t="n">
-        <v>2.07739995598795</v>
-      </c>
-      <c r="K40" s="6" t="n">
+      <c r="J40" s="3">
+        <v>2.0773999559879499</v>
+      </c>
+      <c r="K40" s="6">
         <v>705507</v>
       </c>
-      <c r="L40" s="7" t="s">
-        <v>34</v>
+      <c r="L40" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
@@ -2568,17 +2868,17 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="8" t="n">
+      <c r="C41" s="8">
         <v>24</v>
       </c>
-      <c r="D41" s="4" t="n">
+      <c r="D41" s="4">
         <v>3766</v>
       </c>
       <c r="E41" s="1"/>
@@ -2591,17 +2891,17 @@
       <c r="H41" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I41" s="3" t="n">
+      <c r="I41" s="3">
         <v>3.28</v>
       </c>
-      <c r="J41" s="3" t="n">
+      <c r="J41" s="3">
         <v>1.91199543574383</v>
       </c>
-      <c r="K41" s="6" t="n">
+      <c r="K41" s="6">
         <v>712440</v>
       </c>
-      <c r="L41" s="7" t="s">
-        <v>34</v>
+      <c r="L41" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -2618,17 +2918,17 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="8" t="n">
+      <c r="C42" s="8">
         <v>25</v>
       </c>
-      <c r="D42" s="4" t="n">
+      <c r="D42" s="4">
         <v>3766</v>
       </c>
       <c r="E42" s="1"/>
@@ -2641,17 +2941,17 @@
       <c r="H42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="3" t="n">
+      <c r="I42" s="3">
         <v>3.66</v>
       </c>
-      <c r="J42" s="3" t="n">
-        <v>2.42459739883901</v>
-      </c>
-      <c r="K42" s="6" t="n">
+      <c r="J42" s="3">
+        <v>2.4245973988390102</v>
+      </c>
+      <c r="K42" s="6">
         <v>695047</v>
       </c>
-      <c r="L42" s="7" t="s">
-        <v>34</v>
+      <c r="L42" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -2668,17 +2968,17 @@
       <c r="Y42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="8" t="n">
+      <c r="C43" s="8">
         <v>26</v>
       </c>
-      <c r="D43" s="4" t="n">
+      <c r="D43" s="4">
         <v>3766</v>
       </c>
       <c r="E43" s="1"/>
@@ -2691,17 +2991,17 @@
       <c r="H43" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I43" s="3" t="n">
+      <c r="I43" s="3">
         <v>2.06</v>
       </c>
-      <c r="J43" s="3" t="n">
-        <v>3.05577908119186</v>
-      </c>
-      <c r="K43" s="6" t="n">
+      <c r="J43" s="3">
+        <v>3.0557790811918601</v>
+      </c>
+      <c r="K43" s="6">
         <v>692000</v>
       </c>
-      <c r="L43" s="7" t="s">
-        <v>34</v>
+      <c r="L43" s="11" t="s">
+        <v>106</v>
       </c>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -2718,17 +3018,17 @@
       <c r="Y43" s="1"/>
       <c r="Z43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="8" t="n">
+      <c r="C44" s="8">
         <v>27</v>
       </c>
-      <c r="D44" s="4" t="n">
+      <c r="D44" s="4">
         <v>3766</v>
       </c>
       <c r="E44" s="1"/>
@@ -2741,17 +3041,17 @@
       <c r="H44" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I44" s="3" t="n">
+      <c r="I44" s="3">
         <v>4.26</v>
       </c>
-      <c r="J44" s="3" t="n">
-        <v>1.29936315610826</v>
-      </c>
-      <c r="K44" s="6" t="n">
+      <c r="J44" s="3">
+        <v>1.2993631561082599</v>
+      </c>
+      <c r="K44" s="6">
         <v>608544</v>
       </c>
-      <c r="L44" s="7" t="s">
-        <v>34</v>
+      <c r="L44" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -2768,17 +3068,17 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="8" t="n">
+      <c r="C45" s="8">
         <v>28</v>
       </c>
-      <c r="D45" s="4" t="n">
+      <c r="D45" s="4">
         <v>3766</v>
       </c>
       <c r="E45" s="1"/>
@@ -2791,17 +3091,17 @@
       <c r="H45" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I45" s="3" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="J45" s="3" t="n">
-        <v>1.56305514744716</v>
-      </c>
-      <c r="K45" s="6" t="n">
+      <c r="I45" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J45" s="3">
+        <v>1.5630551474471599</v>
+      </c>
+      <c r="K45" s="6">
         <v>617448</v>
       </c>
-      <c r="L45" s="7" t="s">
-        <v>34</v>
+      <c r="L45" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
@@ -2818,17 +3118,17 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="8" t="n">
+      <c r="C46" s="8">
         <v>29</v>
       </c>
-      <c r="D46" s="4" t="n">
+      <c r="D46" s="4">
         <v>3766</v>
       </c>
       <c r="E46" s="1"/>
@@ -2841,17 +3141,17 @@
       <c r="H46" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I46" s="3" t="n">
+      <c r="I46" s="3">
         <v>1.45</v>
       </c>
-      <c r="J46" s="3" t="n">
-        <v>19.6060465276344</v>
-      </c>
-      <c r="K46" s="6" t="n">
+      <c r="J46" s="3">
+        <v>19.606046527634401</v>
+      </c>
+      <c r="K46" s="6">
         <v>1780106</v>
       </c>
-      <c r="L46" s="7" t="s">
-        <v>34</v>
+      <c r="L46" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
@@ -2868,17 +3168,17 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="8" t="n">
+      <c r="C47" s="8">
         <v>30</v>
       </c>
-      <c r="D47" s="4" t="n">
+      <c r="D47" s="4">
         <v>3766</v>
       </c>
       <c r="E47" s="1"/>
@@ -2891,13 +3191,13 @@
       <c r="H47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="3" t="n">
+      <c r="I47" s="3">
         <v>1.61</v>
       </c>
-      <c r="J47" s="3" t="n">
-        <v>9.89987608049446</v>
-      </c>
-      <c r="K47" s="6" t="n">
+      <c r="J47" s="3">
+        <v>9.8998760804944599</v>
+      </c>
+      <c r="K47" s="6">
         <v>1790455</v>
       </c>
       <c r="L47" s="7" t="s">
@@ -2918,17 +3218,17 @@
       <c r="Y47" s="1"/>
       <c r="Z47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="8" t="n">
+      <c r="C48" s="8">
         <v>31</v>
       </c>
-      <c r="D48" s="4" t="n">
+      <c r="D48" s="4">
         <v>3766</v>
       </c>
       <c r="E48" s="1"/>
@@ -2941,13 +3241,13 @@
       <c r="H48" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I48" s="3" t="n">
+      <c r="I48" s="3">
         <v>1.51</v>
       </c>
-      <c r="J48" s="3" t="n">
+      <c r="J48" s="3">
         <v>12.0536095637591</v>
       </c>
-      <c r="K48" s="6" t="n">
+      <c r="K48" s="6">
         <v>3299346</v>
       </c>
       <c r="L48" s="7" t="s">
@@ -2968,17 +3268,17 @@
       <c r="Y48" s="1"/>
       <c r="Z48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="8" t="n">
+      <c r="C49" s="8">
         <v>32</v>
       </c>
-      <c r="D49" s="4" t="n">
+      <c r="D49" s="4">
         <v>3766</v>
       </c>
       <c r="E49" s="1"/>
@@ -2991,13 +3291,13 @@
       <c r="H49" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I49" s="3" t="n">
+      <c r="I49" s="3">
         <v>1.28</v>
       </c>
-      <c r="J49" s="3" t="n">
-        <v>5.9304527322996</v>
-      </c>
-      <c r="K49" s="6" t="n">
+      <c r="J49" s="3">
+        <v>5.9304527322996003</v>
+      </c>
+      <c r="K49" s="6">
         <v>2258562</v>
       </c>
       <c r="L49" s="7" t="s">
@@ -3018,17 +3318,17 @@
       <c r="Y49" s="1"/>
       <c r="Z49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="8" t="n">
+      <c r="C50" s="8">
         <v>34</v>
       </c>
-      <c r="D50" s="4" t="n">
+      <c r="D50" s="4">
         <v>3766</v>
       </c>
       <c r="E50" s="1"/>
@@ -3041,13 +3341,13 @@
       <c r="H50" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I50" s="3" t="n">
+      <c r="I50" s="3">
         <v>12.3</v>
       </c>
-      <c r="J50" s="3" t="n">
-        <v>0.561908988916423</v>
-      </c>
-      <c r="K50" s="6" t="n">
+      <c r="J50" s="3">
+        <v>0.56190898891642305</v>
+      </c>
+      <c r="K50" s="6">
         <v>608995</v>
       </c>
       <c r="L50" s="7" t="s">
@@ -3068,17 +3368,17 @@
       <c r="Y50" s="1"/>
       <c r="Z50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="9" t="n">
+      <c r="C51" s="9">
         <v>2</v>
       </c>
-      <c r="D51" s="4" t="n">
+      <c r="D51" s="4">
         <v>3766</v>
       </c>
       <c r="E51" s="1"/>
@@ -3091,13 +3391,13 @@
       <c r="H51" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I51" s="3" t="n">
+      <c r="I51" s="3">
         <v>11.9</v>
       </c>
-      <c r="J51" s="3" t="n">
-        <v>0.653643279894271</v>
-      </c>
-      <c r="K51" s="6" t="n">
+      <c r="J51" s="3">
+        <v>0.65364327989427096</v>
+      </c>
+      <c r="K51" s="6">
         <v>3328216</v>
       </c>
       <c r="L51" s="7" t="s">
@@ -3118,17 +3418,17 @@
       <c r="Y51" s="1"/>
       <c r="Z51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C52" s="9" t="n">
+      <c r="C52" s="9">
         <v>5</v>
       </c>
-      <c r="D52" s="4" t="n">
+      <c r="D52" s="4">
         <v>3766</v>
       </c>
       <c r="E52" s="1"/>
@@ -3141,13 +3441,13 @@
       <c r="H52" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I52" s="3" t="n">
+      <c r="I52" s="3">
         <v>3.98</v>
       </c>
-      <c r="J52" s="3" t="n">
-        <v>1.86671618165283</v>
-      </c>
-      <c r="K52" s="6" t="n">
+      <c r="J52" s="3">
+        <v>1.8667161816528299</v>
+      </c>
+      <c r="K52" s="6">
         <v>4261077</v>
       </c>
       <c r="L52" s="7" t="s">
@@ -3168,17 +3468,17 @@
       <c r="Y52" s="1"/>
       <c r="Z52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C53" s="9" t="n">
+      <c r="C53" s="9">
         <v>6</v>
       </c>
-      <c r="D53" s="4" t="n">
+      <c r="D53" s="4">
         <v>3766</v>
       </c>
       <c r="E53" s="1"/>
@@ -3191,13 +3491,13 @@
       <c r="H53" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I53" s="3" t="n">
+      <c r="I53" s="3">
         <v>2.88</v>
       </c>
-      <c r="J53" s="3" t="n">
+      <c r="J53" s="3">
         <v>2.63898957335768</v>
       </c>
-      <c r="K53" s="6" t="n">
+      <c r="K53" s="6">
         <v>3723929</v>
       </c>
       <c r="L53" s="7" t="s">
@@ -3218,17 +3518,17 @@
       <c r="Y53" s="1"/>
       <c r="Z53" s="1"/>
     </row>
-    <row r="54" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="9" t="n">
+      <c r="C54" s="9">
         <v>26</v>
       </c>
-      <c r="D54" s="4" t="n">
+      <c r="D54" s="4">
         <v>3766</v>
       </c>
       <c r="E54" s="1"/>
@@ -3241,13 +3541,13 @@
       <c r="H54" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I54" s="3" t="n">
+      <c r="I54" s="3">
         <v>2.84</v>
       </c>
-      <c r="J54" s="3" t="n">
+      <c r="J54" s="3">
         <v>4.06269027084711</v>
       </c>
-      <c r="K54" s="6" t="n">
+      <c r="K54" s="6">
         <v>6049627</v>
       </c>
       <c r="L54" s="7" t="s">
@@ -3268,17 +3568,17 @@
       <c r="Y54" s="1"/>
       <c r="Z54" s="1"/>
     </row>
-    <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="9" t="n">
+      <c r="C55" s="9">
         <v>27</v>
       </c>
-      <c r="D55" s="4" t="n">
+      <c r="D55" s="4">
         <v>3766</v>
       </c>
       <c r="E55" s="1"/>
@@ -3291,13 +3591,13 @@
       <c r="H55" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I55" s="3" t="n">
+      <c r="I55" s="3">
         <v>2.62</v>
       </c>
-      <c r="J55" s="3" t="n">
-        <v>3.84837632329279</v>
-      </c>
-      <c r="K55" s="6" t="n">
+      <c r="J55" s="3">
+        <v>3.8483763232927899</v>
+      </c>
+      <c r="K55" s="6">
         <v>6156261</v>
       </c>
       <c r="L55" s="7" t="s">
@@ -3318,17 +3618,17 @@
       <c r="Y55" s="1"/>
       <c r="Z55" s="1"/>
     </row>
-    <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="9" t="n">
+      <c r="C56" s="9">
         <v>28</v>
       </c>
-      <c r="D56" s="4" t="n">
+      <c r="D56" s="4">
         <v>3766</v>
       </c>
       <c r="E56" s="1"/>
@@ -3341,13 +3641,13 @@
       <c r="H56" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I56" s="3" t="n">
+      <c r="I56" s="3">
         <v>1.7</v>
       </c>
-      <c r="J56" s="3" t="n">
-        <v>11.2346956109509</v>
-      </c>
-      <c r="K56" s="6" t="n">
+      <c r="J56" s="3">
+        <v>11.234695610950901</v>
+      </c>
+      <c r="K56" s="6">
         <v>6372122</v>
       </c>
       <c r="L56" s="7" t="s">
@@ -3368,17 +3668,17 @@
       <c r="Y56" s="1"/>
       <c r="Z56" s="1"/>
     </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B57" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C57" s="9" t="n">
+      <c r="C57" s="9">
         <v>29</v>
       </c>
-      <c r="D57" s="4" t="n">
+      <c r="D57" s="4">
         <v>3766</v>
       </c>
       <c r="E57" s="1"/>
@@ -3391,13 +3691,13 @@
       <c r="H57" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I57" s="3" t="n">
+      <c r="I57" s="3">
         <v>6.37</v>
       </c>
-      <c r="J57" s="3" t="n">
+      <c r="J57" s="3">
         <v>2.93133594667222</v>
       </c>
-      <c r="K57" s="6" t="n">
+      <c r="K57" s="6">
         <v>8823819</v>
       </c>
       <c r="L57" s="7" t="s">
@@ -3418,17 +3718,17 @@
       <c r="Y57" s="1"/>
       <c r="Z57" s="1"/>
     </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C58" s="9" t="n">
+      <c r="C58" s="9">
         <v>30</v>
       </c>
-      <c r="D58" s="4" t="n">
+      <c r="D58" s="4">
         <v>3766</v>
       </c>
       <c r="E58" s="1"/>
@@ -3441,13 +3741,13 @@
       <c r="H58" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I58" s="3" t="n">
+      <c r="I58" s="3">
         <v>1.62</v>
       </c>
-      <c r="J58" s="3" t="n">
-        <v>7.48754900489457</v>
-      </c>
-      <c r="K58" s="6" t="n">
+      <c r="J58" s="3">
+        <v>7.4875490048945696</v>
+      </c>
+      <c r="K58" s="6">
         <v>6615042</v>
       </c>
       <c r="L58" s="7" t="s">
@@ -3468,17 +3768,17 @@
       <c r="Y58" s="1"/>
       <c r="Z58" s="1"/>
     </row>
-    <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="9" t="n">
+      <c r="C59" s="9">
         <v>7</v>
       </c>
-      <c r="D59" s="4" t="n">
+      <c r="D59" s="4">
         <v>3766</v>
       </c>
       <c r="E59" s="1"/>
@@ -3491,13 +3791,13 @@
       <c r="H59" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I59" s="3" t="n">
+      <c r="I59" s="3">
         <v>18.7</v>
       </c>
-      <c r="J59" s="3" t="n">
-        <v>0.609481033004715</v>
-      </c>
-      <c r="K59" s="6" t="n">
+      <c r="J59" s="3">
+        <v>0.60948103300471501</v>
+      </c>
+      <c r="K59" s="6">
         <v>2851787</v>
       </c>
       <c r="L59" s="7" t="s">
@@ -3518,17 +3818,17 @@
       <c r="Y59" s="1"/>
       <c r="Z59" s="1"/>
     </row>
-    <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="9" t="n">
+      <c r="C60" s="9">
         <v>8</v>
       </c>
-      <c r="D60" s="4" t="n">
+      <c r="D60" s="4">
         <v>3766</v>
       </c>
       <c r="E60" s="1"/>
@@ -3541,13 +3841,13 @@
       <c r="H60" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I60" s="3" t="n">
+      <c r="I60" s="3">
         <v>21.3</v>
       </c>
-      <c r="J60" s="3" t="n">
+      <c r="J60" s="3">
         <v>1.06073797090638</v>
       </c>
-      <c r="K60" s="6" t="n">
+      <c r="K60" s="6">
         <v>3951907</v>
       </c>
       <c r="L60" s="7" t="s">
@@ -3568,17 +3868,17 @@
       <c r="Y60" s="1"/>
       <c r="Z60" s="1"/>
     </row>
-    <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="9" t="n">
+      <c r="C61" s="9">
         <v>9</v>
       </c>
-      <c r="D61" s="4" t="n">
+      <c r="D61" s="4">
         <v>3766</v>
       </c>
       <c r="E61" s="1"/>
@@ -3591,13 +3891,13 @@
       <c r="H61" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I61" s="3" t="n">
+      <c r="I61" s="3">
         <v>2.84</v>
       </c>
-      <c r="J61" s="3" t="n">
-        <v>1.56265852763271</v>
-      </c>
-      <c r="K61" s="6" t="n">
+      <c r="J61" s="3">
+        <v>1.5626585276327101</v>
+      </c>
+      <c r="K61" s="6">
         <v>3774581</v>
       </c>
       <c r="L61" s="7" t="s">
@@ -3618,17 +3918,17 @@
       <c r="Y61" s="1"/>
       <c r="Z61" s="1"/>
     </row>
-    <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="9" t="n">
+      <c r="C62" s="9">
         <v>10</v>
       </c>
-      <c r="D62" s="4" t="n">
+      <c r="D62" s="4">
         <v>3766</v>
       </c>
       <c r="E62" s="1"/>
@@ -3641,13 +3941,13 @@
       <c r="H62" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="3" t="n">
+      <c r="I62" s="3">
         <v>13.5</v>
       </c>
-      <c r="J62" s="3" t="n">
-        <v>0.643620798913658</v>
-      </c>
-      <c r="K62" s="6" t="n">
+      <c r="J62" s="3">
+        <v>0.64362079891365798</v>
+      </c>
+      <c r="K62" s="6">
         <v>2857547</v>
       </c>
       <c r="L62" s="7" t="s">
@@ -3668,17 +3968,17 @@
       <c r="Y62" s="1"/>
       <c r="Z62" s="1"/>
     </row>
-    <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="9" t="n">
+      <c r="C63" s="9">
         <v>11</v>
       </c>
-      <c r="D63" s="4" t="n">
+      <c r="D63" s="4">
         <v>3766</v>
       </c>
       <c r="E63" s="1"/>
@@ -3691,13 +3991,13 @@
       <c r="H63" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I63" s="3" t="n">
-        <v>18.1</v>
-      </c>
-      <c r="J63" s="3" t="n">
-        <v>0.728722229340167</v>
-      </c>
-      <c r="K63" s="6" t="n">
+      <c r="I63" s="3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J63" s="3">
+        <v>0.72872222934016695</v>
+      </c>
+      <c r="K63" s="6">
         <v>7042256</v>
       </c>
       <c r="L63" s="7" t="s">
@@ -3718,17 +4018,17 @@
       <c r="Y63" s="1"/>
       <c r="Z63" s="1"/>
     </row>
-    <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="9" t="n">
+      <c r="C64" s="9">
         <v>12</v>
       </c>
-      <c r="D64" s="4" t="n">
+      <c r="D64" s="4">
         <v>3766</v>
       </c>
       <c r="E64" s="1"/>
@@ -3741,13 +4041,13 @@
       <c r="H64" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I64" s="3" t="n">
+      <c r="I64" s="3">
         <v>46.1</v>
       </c>
-      <c r="J64" s="3" t="n">
-        <v>1.5074680625497</v>
-      </c>
-      <c r="K64" s="6" t="n">
+      <c r="J64" s="3">
+        <v>1.5074680625496999</v>
+      </c>
+      <c r="K64" s="6">
         <v>3562949</v>
       </c>
       <c r="L64" s="7" t="s">
@@ -3768,17 +4068,17 @@
       <c r="Y64" s="1"/>
       <c r="Z64" s="1"/>
     </row>
-    <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B65" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C65" s="9" t="n">
+      <c r="C65" s="9">
         <v>32</v>
       </c>
-      <c r="D65" s="4" t="n">
+      <c r="D65" s="4">
         <v>3766</v>
       </c>
       <c r="E65" s="1"/>
@@ -3791,13 +4091,13 @@
       <c r="H65" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I65" s="3" t="n">
+      <c r="I65" s="3">
         <v>6.18</v>
       </c>
-      <c r="J65" s="3" t="n">
-        <v>0.886643626341421</v>
-      </c>
-      <c r="K65" s="6" t="n">
+      <c r="J65" s="3">
+        <v>0.88664362634142102</v>
+      </c>
+      <c r="K65" s="6">
         <v>3515133</v>
       </c>
       <c r="L65" s="7" t="s">
@@ -3818,17 +4118,17 @@
       <c r="Y65" s="1"/>
       <c r="Z65" s="1"/>
     </row>
-    <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C66" s="9" t="n">
+      <c r="C66" s="9">
         <v>33</v>
       </c>
-      <c r="D66" s="4" t="n">
+      <c r="D66" s="4">
         <v>3766</v>
       </c>
       <c r="E66" s="1"/>
@@ -3841,13 +4141,13 @@
       <c r="H66" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I66" s="3" t="n">
+      <c r="I66" s="3">
         <v>18</v>
       </c>
-      <c r="J66" s="3" t="n">
-        <v>1.28957646525337</v>
-      </c>
-      <c r="K66" s="6" t="n">
+      <c r="J66" s="3">
+        <v>1.2895764652533701</v>
+      </c>
+      <c r="K66" s="6">
         <v>5295291</v>
       </c>
       <c r="L66" s="7" t="s">
@@ -3868,17 +4168,17 @@
       <c r="Y66" s="1"/>
       <c r="Z66" s="1"/>
     </row>
-    <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C67" s="9" t="n">
+      <c r="C67" s="9">
         <v>34</v>
       </c>
-      <c r="D67" s="4" t="n">
+      <c r="D67" s="4">
         <v>3766</v>
       </c>
       <c r="E67" s="1"/>
@@ -3891,13 +4191,13 @@
       <c r="H67" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I67" s="3" t="n">
+      <c r="I67" s="3">
         <v>10.8</v>
       </c>
-      <c r="J67" s="3" t="n">
-        <v>0.890787314017228</v>
-      </c>
-      <c r="K67" s="6" t="n">
+      <c r="J67" s="3">
+        <v>0.89078731401722799</v>
+      </c>
+      <c r="K67" s="6">
         <v>6050621</v>
       </c>
       <c r="L67" s="7" t="s">
@@ -3918,17 +4218,17 @@
       <c r="Y67" s="1"/>
       <c r="Z67" s="1"/>
     </row>
-    <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B68" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C68" s="9" t="n">
+      <c r="C68" s="9">
         <v>35</v>
       </c>
-      <c r="D68" s="4" t="n">
+      <c r="D68" s="4">
         <v>3766</v>
       </c>
       <c r="E68" s="1"/>
@@ -3941,13 +4241,13 @@
       <c r="H68" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I68" s="3" t="n">
+      <c r="I68" s="3">
         <v>26</v>
       </c>
-      <c r="J68" s="3" t="n">
-        <v>0.816432498385129</v>
-      </c>
-      <c r="K68" s="6" t="n">
+      <c r="J68" s="3">
+        <v>0.81643249838512899</v>
+      </c>
+      <c r="K68" s="6">
         <v>5701950</v>
       </c>
       <c r="L68" s="7" t="s">
@@ -3968,17 +4268,17 @@
       <c r="Y68" s="1"/>
       <c r="Z68" s="1"/>
     </row>
-    <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B69" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C69" s="9" t="n">
+      <c r="C69" s="9">
         <v>36</v>
       </c>
-      <c r="D69" s="4" t="n">
+      <c r="D69" s="4">
         <v>3766</v>
       </c>
       <c r="E69" s="1"/>
@@ -3991,13 +4291,13 @@
       <c r="H69" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I69" s="3" t="n">
+      <c r="I69" s="3">
         <v>2.02</v>
       </c>
-      <c r="J69" s="3" t="n">
-        <v>5.90413437443556</v>
-      </c>
-      <c r="K69" s="6" t="n">
+      <c r="J69" s="3">
+        <v>5.9041343744355599</v>
+      </c>
+      <c r="K69" s="6">
         <v>5646144</v>
       </c>
       <c r="L69" s="7" t="s">
@@ -4018,17 +4318,17 @@
       <c r="Y69" s="1"/>
       <c r="Z69" s="1"/>
     </row>
-    <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="9" t="n">
-        <v>13</v>
-      </c>
-      <c r="D70" s="4" t="n">
+      <c r="C70" s="9">
+        <v>13</v>
+      </c>
+      <c r="D70" s="4">
         <v>3766</v>
       </c>
       <c r="E70" s="1"/>
@@ -4041,13 +4341,13 @@
       <c r="H70" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I70" s="3" t="n">
-        <v>16.9</v>
-      </c>
-      <c r="J70" s="3" t="n">
-        <v>0.858517283018868</v>
-      </c>
-      <c r="K70" s="6" t="n">
+      <c r="I70" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J70" s="3">
+        <v>0.85851728301886798</v>
+      </c>
+      <c r="K70" s="6">
         <v>3830700</v>
       </c>
       <c r="L70" s="7" t="s">
@@ -4068,17 +4368,17 @@
       <c r="Y70" s="1"/>
       <c r="Z70" s="1"/>
     </row>
-    <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="9" t="n">
-        <v>14</v>
-      </c>
-      <c r="D71" s="4" t="n">
+      <c r="C71" s="9">
+        <v>14</v>
+      </c>
+      <c r="D71" s="4">
         <v>3766</v>
       </c>
       <c r="E71" s="1"/>
@@ -4091,13 +4391,13 @@
       <c r="H71" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I71" s="3" t="n">
+      <c r="I71" s="3">
         <v>18.5</v>
       </c>
-      <c r="J71" s="3" t="n">
-        <v>0.616349913307326</v>
-      </c>
-      <c r="K71" s="6" t="n">
+      <c r="J71" s="3">
+        <v>0.61634991330732602</v>
+      </c>
+      <c r="K71" s="6">
         <v>1649598</v>
       </c>
       <c r="L71" s="7" t="s">
@@ -4118,17 +4418,17 @@
       <c r="Y71" s="1"/>
       <c r="Z71" s="1"/>
     </row>
-    <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="D72" s="4" t="n">
+      <c r="C72" s="9">
+        <v>15</v>
+      </c>
+      <c r="D72" s="4">
         <v>3766</v>
       </c>
       <c r="E72" s="1"/>
@@ -4141,13 +4441,13 @@
       <c r="H72" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I72" s="3" t="n">
+      <c r="I72" s="3">
         <v>3.31</v>
       </c>
-      <c r="J72" s="3" t="n">
-        <v>2.93706763514157</v>
-      </c>
-      <c r="K72" s="6" t="n">
+      <c r="J72" s="3">
+        <v>2.9370676351415699</v>
+      </c>
+      <c r="K72" s="6">
         <v>3475585</v>
       </c>
       <c r="L72" s="7" t="s">
@@ -4168,17 +4468,17 @@
       <c r="Y72" s="1"/>
       <c r="Z72" s="1"/>
     </row>
-    <row r="73" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C73" s="9" t="n">
-        <v>16</v>
-      </c>
-      <c r="D73" s="4" t="n">
+      <c r="C73" s="9">
+        <v>16</v>
+      </c>
+      <c r="D73" s="4">
         <v>3766</v>
       </c>
       <c r="E73" s="1"/>
@@ -4191,13 +4491,13 @@
       <c r="H73" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I73" s="3" t="n">
+      <c r="I73" s="3">
         <v>4.34</v>
       </c>
-      <c r="J73" s="3" t="n">
-        <v>3.34701737805614</v>
-      </c>
-      <c r="K73" s="6" t="n">
+      <c r="J73" s="3">
+        <v>3.3470173780561399</v>
+      </c>
+      <c r="K73" s="6">
         <v>3535194</v>
       </c>
       <c r="L73" s="7" t="s">
@@ -4218,17 +4518,17 @@
       <c r="Y73" s="1"/>
       <c r="Z73" s="1"/>
     </row>
-    <row r="74" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="9" t="n">
+      <c r="C74" s="9">
         <v>17</v>
       </c>
-      <c r="D74" s="4" t="n">
+      <c r="D74" s="4">
         <v>3766</v>
       </c>
       <c r="E74" s="1"/>
@@ -4241,13 +4541,13 @@
       <c r="H74" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I74" s="3" t="n">
+      <c r="I74" s="3">
         <v>2.73</v>
       </c>
-      <c r="J74" s="3" t="n">
+      <c r="J74" s="3">
         <v>2.44358218214657</v>
       </c>
-      <c r="K74" s="6" t="n">
+      <c r="K74" s="6">
         <v>1702672</v>
       </c>
       <c r="L74" s="7" t="s">
@@ -4268,17 +4568,17 @@
       <c r="Y74" s="1"/>
       <c r="Z74" s="1"/>
     </row>
-    <row r="75" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C75" s="9" t="n">
+      <c r="C75" s="9">
         <v>18</v>
       </c>
-      <c r="D75" s="4" t="n">
+      <c r="D75" s="4">
         <v>3766</v>
       </c>
       <c r="E75" s="1"/>
@@ -4291,13 +4591,13 @@
       <c r="H75" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I75" s="3" t="n">
+      <c r="I75" s="3">
         <v>7.93</v>
       </c>
-      <c r="J75" s="3" t="n">
-        <v>1.27361348673843</v>
-      </c>
-      <c r="K75" s="6" t="n">
+      <c r="J75" s="3">
+        <v>1.2736134867384299</v>
+      </c>
+      <c r="K75" s="6">
         <v>2553094</v>
       </c>
       <c r="L75" s="7" t="s">
@@ -4318,17 +4618,17 @@
       <c r="Y75" s="1"/>
       <c r="Z75" s="1"/>
     </row>
-    <row r="76" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B76" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C76" s="9" t="n">
+      <c r="C76" s="9">
         <v>37</v>
       </c>
-      <c r="D76" s="4" t="n">
+      <c r="D76" s="4">
         <v>3766</v>
       </c>
       <c r="E76" s="1"/>
@@ -4341,13 +4641,13 @@
       <c r="H76" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I76" s="3" t="n">
+      <c r="I76" s="3">
         <v>1.73</v>
       </c>
-      <c r="J76" s="3" t="n">
-        <v>4.72672642725036</v>
-      </c>
-      <c r="K76" s="6" t="n">
+      <c r="J76" s="3">
+        <v>4.7267264272503597</v>
+      </c>
+      <c r="K76" s="6">
         <v>6526380</v>
       </c>
       <c r="L76" s="7" t="s">
@@ -4368,17 +4668,17 @@
       <c r="Y76" s="1"/>
       <c r="Z76" s="1"/>
     </row>
-    <row r="77" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B77" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C77" s="9" t="n">
+      <c r="C77" s="9">
         <v>38</v>
       </c>
-      <c r="D77" s="4" t="n">
+      <c r="D77" s="4">
         <v>3766</v>
       </c>
       <c r="E77" s="1"/>
@@ -4391,13 +4691,13 @@
       <c r="H77" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I77" s="3" t="n">
+      <c r="I77" s="3">
         <v>5.43</v>
       </c>
-      <c r="J77" s="3" t="n">
-        <v>0.960835048212147</v>
-      </c>
-      <c r="K77" s="6" t="n">
+      <c r="J77" s="3">
+        <v>0.96083504821214705</v>
+      </c>
+      <c r="K77" s="6">
         <v>5766569</v>
       </c>
       <c r="L77" s="7" t="s">
@@ -4418,17 +4718,17 @@
       <c r="Y77" s="1"/>
       <c r="Z77" s="1"/>
     </row>
-    <row r="78" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="9" t="n">
+      <c r="C78" s="9">
         <v>39</v>
       </c>
-      <c r="D78" s="4" t="n">
+      <c r="D78" s="4">
         <v>3766</v>
       </c>
       <c r="E78" s="1"/>
@@ -4441,13 +4741,13 @@
       <c r="H78" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I78" s="3" t="n">
-        <v>8.97</v>
-      </c>
-      <c r="J78" s="3" t="n">
-        <v>1.66315463201564</v>
-      </c>
-      <c r="K78" s="6" t="n">
+      <c r="I78" s="3">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="J78" s="3">
+        <v>1.6631546320156401</v>
+      </c>
+      <c r="K78" s="6">
         <v>5255348</v>
       </c>
       <c r="L78" s="7" t="s">
@@ -4468,17 +4768,17 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B79" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="9" t="n">
+      <c r="C79" s="9">
         <v>40</v>
       </c>
-      <c r="D79" s="4" t="n">
+      <c r="D79" s="4">
         <v>3766</v>
       </c>
       <c r="E79" s="1"/>
@@ -4491,13 +4791,13 @@
       <c r="H79" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I79" s="3" t="n">
+      <c r="I79" s="3">
         <v>2.02</v>
       </c>
-      <c r="J79" s="3" t="n">
-        <v>4.2277502750275</v>
-      </c>
-      <c r="K79" s="6" t="n">
+      <c r="J79" s="3">
+        <v>4.2277502750274998</v>
+      </c>
+      <c r="K79" s="6">
         <v>3622867</v>
       </c>
       <c r="L79" s="7" t="s">
@@ -4518,17 +4818,17 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B80" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C80" s="9" t="n">
+      <c r="C80" s="9">
         <v>42</v>
       </c>
-      <c r="D80" s="4" t="n">
+      <c r="D80" s="4">
         <v>3766</v>
       </c>
       <c r="E80" s="1"/>
@@ -4541,13 +4841,13 @@
       <c r="H80" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I80" s="3" t="n">
+      <c r="I80" s="3">
         <v>9.18</v>
       </c>
-      <c r="J80" s="3" t="n">
+      <c r="J80" s="3">
         <v>1.3482159894507</v>
       </c>
-      <c r="K80" s="6" t="n">
+      <c r="K80" s="6">
         <v>4651995</v>
       </c>
       <c r="L80" s="7" t="s">
@@ -4568,17 +4868,17 @@
       <c r="Y80" s="1"/>
       <c r="Z80" s="1"/>
     </row>
-    <row r="81" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="9" t="n">
+      <c r="C81" s="9">
         <v>19</v>
       </c>
-      <c r="D81" s="4" t="n">
+      <c r="D81" s="4">
         <v>3766</v>
       </c>
       <c r="E81" s="1"/>
@@ -4591,13 +4891,13 @@
       <c r="H81" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I81" s="3" t="n">
+      <c r="I81" s="3">
         <v>4.92</v>
       </c>
-      <c r="J81" s="3" t="n">
-        <v>1.78675720335256</v>
-      </c>
-      <c r="K81" s="6" t="n">
+      <c r="J81" s="3">
+        <v>1.7867572033525601</v>
+      </c>
+      <c r="K81" s="6">
         <v>3865665</v>
       </c>
       <c r="L81" s="7" t="s">
@@ -4618,17 +4918,17 @@
       <c r="Y81" s="1"/>
       <c r="Z81" s="1"/>
     </row>
-    <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C82" s="9" t="n">
+      <c r="C82" s="9">
         <v>20</v>
       </c>
-      <c r="D82" s="4" t="n">
+      <c r="D82" s="4">
         <v>3766</v>
       </c>
       <c r="E82" s="1"/>
@@ -4641,13 +4941,13 @@
       <c r="H82" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I82" s="3" t="n">
-        <v>18.1</v>
-      </c>
-      <c r="J82" s="3" t="n">
-        <v>0.642639059940117</v>
-      </c>
-      <c r="K82" s="6" t="n">
+      <c r="I82" s="3">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="J82" s="3">
+        <v>0.64263905994011705</v>
+      </c>
+      <c r="K82" s="6">
         <v>1469460</v>
       </c>
       <c r="L82" s="7" t="s">
@@ -4668,17 +4968,17 @@
       <c r="Y82" s="1"/>
       <c r="Z82" s="1"/>
     </row>
-    <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="9" t="n">
+      <c r="C83" s="9">
         <v>22</v>
       </c>
-      <c r="D83" s="4" t="n">
+      <c r="D83" s="4">
         <v>3766</v>
       </c>
       <c r="E83" s="1"/>
@@ -4691,13 +4991,13 @@
       <c r="H83" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I83" s="3" t="n">
+      <c r="I83" s="3">
         <v>21.6</v>
       </c>
-      <c r="J83" s="3" t="n">
-        <v>0.44670543883762</v>
-      </c>
-      <c r="K83" s="6" t="n">
+      <c r="J83" s="3">
+        <v>0.44670543883761998</v>
+      </c>
+      <c r="K83" s="6">
         <v>3665601</v>
       </c>
       <c r="L83" s="7" t="s">
@@ -4718,17 +5018,17 @@
       <c r="Y83" s="1"/>
       <c r="Z83" s="1"/>
     </row>
-    <row r="84" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C84" s="9" t="n">
+      <c r="C84" s="9">
         <v>23</v>
       </c>
-      <c r="D84" s="4" t="n">
+      <c r="D84" s="4">
         <v>3766</v>
       </c>
       <c r="E84" s="1"/>
@@ -4741,13 +5041,13 @@
       <c r="H84" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I84" s="3" t="n">
+      <c r="I84" s="3">
         <v>15.5</v>
       </c>
-      <c r="J84" s="3" t="n">
-        <v>0.824420495724018</v>
-      </c>
-      <c r="K84" s="6" t="n">
+      <c r="J84" s="3">
+        <v>0.82442049572401799</v>
+      </c>
+      <c r="K84" s="6">
         <v>3528108</v>
       </c>
       <c r="L84" s="7" t="s">
@@ -4768,17 +5068,17 @@
       <c r="Y84" s="1"/>
       <c r="Z84" s="1"/>
     </row>
-    <row r="85" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="9" t="n">
+      <c r="C85" s="9">
         <v>24</v>
       </c>
-      <c r="D85" s="4" t="n">
+      <c r="D85" s="4">
         <v>3766</v>
       </c>
       <c r="E85" s="1"/>
@@ -4791,13 +5091,13 @@
       <c r="H85" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I85" s="3" t="n">
+      <c r="I85" s="3">
         <v>45.8</v>
       </c>
-      <c r="J85" s="3" t="n">
+      <c r="J85" s="3">
         <v>0.948262254084695</v>
       </c>
-      <c r="K85" s="6" t="n">
+      <c r="K85" s="6">
         <v>3343546</v>
       </c>
       <c r="L85" s="7" t="s">
@@ -4818,17 +5118,17 @@
       <c r="Y85" s="1"/>
       <c r="Z85" s="1"/>
     </row>
-    <row r="86" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B86" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C86" s="9" t="n">
+      <c r="C86" s="9">
         <v>43</v>
       </c>
-      <c r="D86" s="4" t="n">
+      <c r="D86" s="4">
         <v>3766</v>
       </c>
       <c r="E86" s="1"/>
@@ -4841,13 +5141,13 @@
       <c r="H86" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I86" s="3" t="n">
-        <v>17.6</v>
-      </c>
-      <c r="J86" s="3" t="n">
-        <v>0.965895728963234</v>
-      </c>
-      <c r="K86" s="6" t="n">
+      <c r="I86" s="3">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J86" s="3">
+        <v>0.96589572896323395</v>
+      </c>
+      <c r="K86" s="6">
         <v>4085190</v>
       </c>
       <c r="L86" s="7" t="s">
@@ -4868,17 +5168,17 @@
       <c r="Y86" s="1"/>
       <c r="Z86" s="1"/>
     </row>
-    <row r="87" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B87" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C87" s="9" t="n">
+      <c r="C87" s="9">
         <v>44</v>
       </c>
-      <c r="D87" s="4" t="n">
+      <c r="D87" s="4">
         <v>3766</v>
       </c>
       <c r="E87" s="1"/>
@@ -4891,13 +5191,13 @@
       <c r="H87" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I87" s="3" t="n">
-        <v>40.7</v>
-      </c>
-      <c r="J87" s="3" t="n">
+      <c r="I87" s="3">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="J87" s="3">
         <v>1.06891129486939</v>
       </c>
-      <c r="K87" s="6" t="n">
+      <c r="K87" s="6">
         <v>1835789</v>
       </c>
       <c r="L87" s="7" t="s">
@@ -4918,17 +5218,17 @@
       <c r="Y87" s="1"/>
       <c r="Z87" s="1"/>
     </row>
-    <row r="88" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B88" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C88" s="9" t="n">
+      <c r="C88" s="9">
         <v>45</v>
       </c>
-      <c r="D88" s="4" t="n">
+      <c r="D88" s="4">
         <v>3766</v>
       </c>
       <c r="E88" s="1"/>
@@ -4941,13 +5241,13 @@
       <c r="H88" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I88" s="3" t="n">
+      <c r="I88" s="3">
         <v>4.79</v>
       </c>
-      <c r="J88" s="3" t="n">
+      <c r="J88" s="3">
         <v>1.99095652551355</v>
       </c>
-      <c r="K88" s="6" t="n">
+      <c r="K88" s="6">
         <v>4797731</v>
       </c>
       <c r="L88" s="7" t="s">
@@ -4968,17 +5268,17 @@
       <c r="Y88" s="1"/>
       <c r="Z88" s="1"/>
     </row>
-    <row r="89" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B89" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C89" s="9" t="n">
+      <c r="C89" s="9">
         <v>46</v>
       </c>
-      <c r="D89" s="4" t="n">
+      <c r="D89" s="4">
         <v>3766</v>
       </c>
       <c r="E89" s="1"/>
@@ -4991,13 +5291,13 @@
       <c r="H89" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I89" s="3" t="n">
+      <c r="I89" s="3">
         <v>9.76</v>
       </c>
-      <c r="J89" s="3" t="n">
+      <c r="J89" s="3">
         <v>1.38982540182115</v>
       </c>
-      <c r="K89" s="6" t="n">
+      <c r="K89" s="6">
         <v>6135527</v>
       </c>
       <c r="L89" s="7" t="s">
@@ -5018,17 +5318,17 @@
       <c r="Y89" s="1"/>
       <c r="Z89" s="1"/>
     </row>
-    <row r="90" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B90" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C90" s="9" t="n">
+      <c r="C90" s="9">
         <v>47</v>
       </c>
-      <c r="D90" s="4" t="n">
+      <c r="D90" s="4">
         <v>3766</v>
       </c>
       <c r="E90" s="1"/>
@@ -5041,13 +5341,13 @@
       <c r="H90" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I90" s="3" t="n">
+      <c r="I90" s="3">
         <v>15.2</v>
       </c>
-      <c r="J90" s="3" t="n">
-        <v>1.43537589905363</v>
-      </c>
-      <c r="K90" s="6" t="n">
+      <c r="J90" s="3">
+        <v>1.4353758990536301</v>
+      </c>
+      <c r="K90" s="6">
         <v>3991778</v>
       </c>
       <c r="L90" s="7" t="s">
@@ -5068,17 +5368,17 @@
       <c r="Y90" s="1"/>
       <c r="Z90" s="1"/>
     </row>
-    <row r="91" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B91" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="C91" s="9" t="n">
+      <c r="C91" s="9">
         <v>48</v>
       </c>
-      <c r="D91" s="4" t="n">
+      <c r="D91" s="4">
         <v>3766</v>
       </c>
       <c r="E91" s="1"/>
@@ -5091,13 +5391,13 @@
       <c r="H91" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I91" s="3" t="n">
-        <v>16.4</v>
-      </c>
-      <c r="J91" s="3" t="n">
-        <v>1.18382287438859</v>
-      </c>
-      <c r="K91" s="6" t="n">
+      <c r="I91" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J91" s="3">
+        <v>1.1838228743885899</v>
+      </c>
+      <c r="K91" s="6">
         <v>5270337</v>
       </c>
       <c r="L91" s="7" t="s">
@@ -5119,12 +5419,7 @@
       <c r="Z91" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>